<commit_message>
Thêm sheet lịch sử thay đổi
</commit_message>
<xml_diff>
--- a/Documents/Design/SequenceDiagram.xlsx
+++ b/Documents/Design/SequenceDiagram.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>QUẢN LÍ KHAI SINH</t>
   </si>
@@ -57,16 +57,13 @@
     <t>Nguyễn Phạm Anh Thư</t>
   </si>
   <si>
-    <t>31/03/2017</t>
-  </si>
-  <si>
-    <t>Thiết kế WorkFlow, Use Case</t>
-  </si>
-  <si>
     <t>Trang Phương Trúc</t>
   </si>
   <si>
     <t>Bổ sung Sheet Lịch sử thay đổi</t>
+  </si>
+  <si>
+    <t>Thiết kế Sequence Diagram</t>
   </si>
 </sst>
 </file>
@@ -336,6 +333,34 @@
     <xf numFmtId="14" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -352,34 +377,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -725,39 +722,39 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="26"/>
-    <col min="2" max="2" width="12" style="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="26"/>
-    <col min="4" max="4" width="12" style="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="26"/>
+    <col min="1" max="1" width="9.140625" style="16"/>
+    <col min="2" max="2" width="12" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="16"/>
+    <col min="4" max="4" width="12" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:11" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="17"/>
-    </row>
-    <row r="2" spans="1:11" s="18" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="10"/>
+    </row>
+    <row r="2" spans="1:11" s="11" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -765,203 +762,235 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-      <c r="K2" s="20"/>
-    </row>
-    <row r="3" spans="1:11" s="23" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="21" t="s">
+      <c r="K2" s="12"/>
+    </row>
+    <row r="3" spans="1:11" s="14" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22" t="s">
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22" t="s">
+      <c r="F3" s="21"/>
+      <c r="G3" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="24">
+      <c r="A4" s="15">
         <v>1</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25" t="s">
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="18">
+        <v>42770</v>
+      </c>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="15">
+        <v>2</v>
+      </c>
+      <c r="B5" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25" t="s">
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="18">
+        <v>42798</v>
+      </c>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="25"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="24">
-        <v>2</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="27">
-        <v>42798</v>
-      </c>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
+      <c r="A6" s="15"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
+      <c r="A7" s="15"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="25"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25"/>
+      <c r="A11" s="15"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="24"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="24"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="25"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="24"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="25"/>
+      <c r="A14" s="15"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
+      <c r="A15" s="15"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:K4"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:K3"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:K5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:K6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:K10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:K11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:K12"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="E15:F15"/>
     <mergeCell ref="G15:K15"/>
@@ -971,38 +1000,6 @@
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="G14:K14"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:K11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:K12"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:K9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:K10"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:K7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:K5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:K6"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:K3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:K4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1012,8 +1009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP117"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1024,31 +1021,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="24"/>
+      <c r="C2" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="15"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="27"/>
       <c r="H2" s="4" t="s">
         <v>1</v>
       </c>

</xml_diff>